<commit_message>
Increased items to 101.
</commit_message>
<xml_diff>
--- a/capitals.xlsx
+++ b/capitals.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cia/Desktop/github/user-models-group-project-team-apple/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ckyri\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5858550D-8CD0-6B47-BE98-B47B107A4D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE64AA8D-4901-4849-97CE-E1F16D8EC4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{177B1AFC-5F33-4CF4-BA8D-79994B715521}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{177B1AFC-5F33-4CF4-BA8D-79994B715521}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="436">
   <si>
     <t>fact_id</t>
   </si>
@@ -344,9 +344,6 @@
     <t>cyprus</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>nicosia</t>
   </si>
   <si>
@@ -458,9 +455,6 @@
     <t>question_context</t>
   </si>
   <si>
-    <t>none</t>
-  </si>
-  <si>
     <t>St. John’s has one of the major cruise ship ports in the Eastern Caribbean.</t>
   </si>
   <si>
@@ -632,10 +626,725 @@
     <t>Zimbabwe has 8 different currencies in circulation, but the US dollar is most commonly used in Harare.</t>
   </si>
   <si>
-    <t>Andorra la Vella is the highest capital city in Europe, located at an elevation of 1,023 meters (3,356 feet) above sea level.</t>
-  </si>
-  <si>
-    <t>Vienna is the world capital of waltz; as many as 450 balls are organized in the city annually, especially during january and february. the famous “requiem” of Mozart sounds the best (according to music experts) when performed in St. Stephen’s cathedral in Vienna.</t>
+    <t>What Eastern Caribbean capital is known for hosting one of the major cruise ship ports?</t>
+  </si>
+  <si>
+    <t>Which capital is famous for its exceptionally clear ocean waters where you can see up to 200 feet below the surface?</t>
+  </si>
+  <si>
+    <t>What UNESCO world heritage site capital showcases British colonial architecture and is home to the Barbados parliament buildings?</t>
+  </si>
+  <si>
+    <t>Which is the smallest capital in Central America (in terms of population)?</t>
+  </si>
+  <si>
+    <t>What national capital ranks as the second coldest globally and features the world's longest ice skating rink in winter</t>
+  </si>
+  <si>
+    <t>What capital is renowned for its continued use of classic cars from the 1950s, as a result of trade restrictions during the U.S. embargo in 1962?</t>
+  </si>
+  <si>
+    <t>Which capital city has no army since 1948?</t>
+  </si>
+  <si>
+    <t>Which capital, located on the "nature island," is surrounded by lush rainforests and natural beauty?</t>
+  </si>
+  <si>
+    <t>What capital holds the distinction of being the oldest city in the Americas colonized by Europeans?</t>
+  </si>
+  <si>
+    <t>Which capital is situated in a volcanic valley and is prone to earthquakes?</t>
+  </si>
+  <si>
+    <t>What is the largest city in Central America?</t>
+  </si>
+  <si>
+    <t>Which capital is famous for its spice productions?</t>
+  </si>
+  <si>
+    <t>Which capital saw its national palace severely damaged by an earthquake in 2010, with the remnants serving as a reminder of this disaster?</t>
+  </si>
+  <si>
+    <t>What capital became the permanent capital in 1880 and was later combined with Comayagüela in 1938?</t>
+  </si>
+  <si>
+    <t>Which capital is celebrated as the birthplace of reggae music and houses the popular Bob Marley museum?</t>
+  </si>
+  <si>
+    <t>What capital is constructed on the ruins of the ancient Aztec city of Tenochtitlán?</t>
+  </si>
+  <si>
+    <t>What capital is known for its "Ruins of the Old Cathedral," which was damaged in an earthquake and never restored?</t>
+  </si>
+  <si>
+    <t>Which capital features a modern skyline that with the original city founded by the Spanish in 1519?</t>
+  </si>
+  <si>
+    <t>Which capital is home to the independence square, once the site of slave auctions and now a symbol of the nation's independence?</t>
+  </si>
+  <si>
+    <t>Which capital's name is still a mystery until today?</t>
+  </si>
+  <si>
+    <t>Which european capital city is situated at the highest elevation, at 1,023 meters above sea level?</t>
+  </si>
+  <si>
+    <t>What capital is known as the world capital of waltz, and for the performance of mozart's "requiem" taking place in St. Stephen's Cathedral?</t>
+  </si>
+  <si>
+    <t>Which capital was home to the largest Jewish ghetto in the Soviet territory during World War II?</t>
+  </si>
+  <si>
+    <t>Which capital city houses the world's largest outlet for chocolate sales at its airport?</t>
+  </si>
+  <si>
+    <t>In which capital did the assassination of Archduke Franz Ferdinand take place, leading to the events that sparked World War I?</t>
+  </si>
+  <si>
+    <t>What capital boasts a metro system with stations decorated with archaeological artifacts discovered during construction?</t>
+  </si>
+  <si>
+    <t>Which capital features the world's shortest public transport vehicle ride?</t>
+  </si>
+  <si>
+    <t>What capital city is known as the last divided capital, with a "green line" separating the Greek Cypriot south and the Turkish Cypriot north?</t>
+  </si>
+  <si>
+    <t>Which capital is home to the renowned astronomical clock, which has been continuously operating since its installation in 1410??</t>
+  </si>
+  <si>
+    <t>What capital is famous for its cycling culture, with more bicycles than people residing in the city?</t>
+  </si>
+  <si>
+    <t>Which capital is one of the best-preserved medieval towns in Europe, designated as a UNESCO World Heritage site?</t>
+  </si>
+  <si>
+    <t>Which Nordic capital city has the coldest average winter temperature among the five main Nordic capitals?</t>
+  </si>
+  <si>
+    <t>What capital city's name means "high ground" or "mountain stronghold," and it is strategically located, surrounded by mountains?</t>
+  </si>
+  <si>
+    <t>Which capital is characterized by its picturesque pink-hued buildings made of volcanic tufa stone?</t>
+  </si>
+  <si>
+    <t>Which capital is renowned for its three futuristic skyscrapers known as the flame towers?</t>
+  </si>
+  <si>
+    <t>What capital is closely located to Dive Bahrain, an underwater theme park featuring a sunken Boeing 747</t>
+  </si>
+  <si>
+    <t>In which capital can one find thriving textile industries such as jute, muslin, and cotton, where people buy cloth and order custom-made clothes at affordable prices?</t>
+  </si>
+  <si>
+    <t>Which unique capital city operates without traffic lights and relies on traffic police using hand signals to manage traffic?</t>
+  </si>
+  <si>
+    <t>Which capital is a blend of two terrains, with some parts being on dry land and others extending into the sea?</t>
+  </si>
+  <si>
+    <t>Which capital is known as the 'pearl of Asia'?</t>
+  </si>
+  <si>
+    <t>Which capital city houses the Forbidden City?</t>
+  </si>
+  <si>
+    <t>What capital's existence is owed to underground thermal waters according to a legend?</t>
+  </si>
+  <si>
+    <t>This capital is often confused with the city within which the capital is found?</t>
+  </si>
+  <si>
+    <t>Which capital's name is of Portuguese origin, meaning "Saint Thomas"?</t>
+  </si>
+  <si>
+    <t>In which capital did singer Akon spend his childhood?</t>
+  </si>
+  <si>
+    <t>Which capital city is known for being the world's smallest, both in terms of land area and population?</t>
+  </si>
+  <si>
+    <t>What capital city features the historic cotton tree?</t>
+  </si>
+  <si>
+    <t>In which capital did the Battle of Mogadishu take place, marking the conclusion of a U.S.-led military intervention in Somalia?</t>
+  </si>
+  <si>
+    <t>What capital city is nicknamed "the jacaranda city" due to its beautiful blooming jacaranda trees with striking purple flowers?</t>
+  </si>
+  <si>
+    <t>Which city is recognized as the world's youngest capital?</t>
+  </si>
+  <si>
+    <t>What capital city serves as the confluence point of the Blue Nile and White Nile rivers, creating the Nile river proper, an area referred to as the "two Niles"?</t>
+  </si>
+  <si>
+    <t>What city was confirmed as the capital  in 1996 after the government's decision to relocate the federal capital from Dar Es Salaam?</t>
+  </si>
+  <si>
+    <t>Which capital city was chosen as the colonial capital of German Togoland in 1897?</t>
+  </si>
+  <si>
+    <t>Which capital is the sole location in Tunisia with a tube service, while other areas rely on coach, public bus, and taxi services?</t>
+  </si>
+  <si>
+    <t>Which capital is known for providing a stunning view of itself from the gaddafi mosque?</t>
+  </si>
+  <si>
+    <t>In which capital is the U.S. dollar the predominant currency?</t>
+  </si>
+  <si>
+    <t>Which capital is famous for the preservation of rare white rhino species?</t>
+  </si>
+  <si>
+    <t>oceania</t>
+  </si>
+  <si>
+    <t>Canberra's layout was designed by an American architect, Walter Burley Griffin, who won an international competition for the city's design.</t>
+  </si>
+  <si>
+    <t>Suva is home to a vibrant arts and crafts scene. Local artisans create intricate traditional handicrafts, including pottery, woodcarvings, and woven baskets.</t>
+  </si>
+  <si>
+    <t>South Tarawa is the capital of Kiribati, an island nation particularly vulnerable to rising sea levels due to climate change.</t>
+  </si>
+  <si>
+    <t>Majuro is not only the capital but also the largest atoll in the Marshall Islands, known for its picturesque lagoon.</t>
+  </si>
+  <si>
+    <t>Palikir serves as the capital of the Federated States of Micronesia and is a central hub for the country's government.</t>
+  </si>
+  <si>
+    <t>Yaren is not officially a capital but serves as the de facto capital of Nauru, a tiny island country in Micronesia, northeast of Australia.</t>
+  </si>
+  <si>
+    <t>Wellington was named after Arthur Wellesley, the first Duke of Wellington who had never been to New Zealand.</t>
+  </si>
+  <si>
+    <t>Ngerulmud is the world's second-youngest capital city, officially declared the capital of Palau in 2006.</t>
+  </si>
+  <si>
+    <t>Port Moresby is the capital of Papua New Guinea and it was named after Captain John Moresby who explored it in 1873.</t>
+  </si>
+  <si>
+    <t>Apia is the capital city of Samoa. The city was originally a small village from which it took its name.</t>
+  </si>
+  <si>
+    <t>Nuku'alofa is the capital of the only remaining monarchy in the Pacific and offers insights into Tonga's rich history.</t>
+  </si>
+  <si>
+    <t>Funafuti was named after a local tribe that inhabited the land before Europeans discovered it.</t>
+  </si>
+  <si>
+    <t>Port Vila is known for its stunning natural beauty and offers various outdoor activities for visitors.</t>
+  </si>
+  <si>
+    <t>australia</t>
+  </si>
+  <si>
+    <t>fiji</t>
+  </si>
+  <si>
+    <t>kiribati</t>
+  </si>
+  <si>
+    <t>marshall Islands</t>
+  </si>
+  <si>
+    <t>micronesia</t>
+  </si>
+  <si>
+    <t>nauru</t>
+  </si>
+  <si>
+    <t>new zealand</t>
+  </si>
+  <si>
+    <t>palau</t>
+  </si>
+  <si>
+    <t>papua new guinea</t>
+  </si>
+  <si>
+    <t>samoa</t>
+  </si>
+  <si>
+    <t>solomon islands</t>
+  </si>
+  <si>
+    <t>tonga</t>
+  </si>
+  <si>
+    <t>tuvalu</t>
+  </si>
+  <si>
+    <t>vanuatu</t>
+  </si>
+  <si>
+    <t>Prior to World War II, this capital did not exist. It developed around the site of the U.S. military headquarters. In 1952 it officially replaced Tulagi as the country's capital.</t>
+  </si>
+  <si>
+    <t>Which capital did not exist before WWII?</t>
+  </si>
+  <si>
+    <t>canberra</t>
+  </si>
+  <si>
+    <t>suva</t>
+  </si>
+  <si>
+    <t>south tarawa</t>
+  </si>
+  <si>
+    <t>majuro</t>
+  </si>
+  <si>
+    <t>palikir</t>
+  </si>
+  <si>
+    <t>yaren</t>
+  </si>
+  <si>
+    <t>wellington</t>
+  </si>
+  <si>
+    <t>ngerulmud</t>
+  </si>
+  <si>
+    <t>port moresby</t>
+  </si>
+  <si>
+    <t>apia</t>
+  </si>
+  <si>
+    <t>honiara</t>
+  </si>
+  <si>
+    <t>nuku'alofa</t>
+  </si>
+  <si>
+    <t>funafuti</t>
+  </si>
+  <si>
+    <t>port vila</t>
+  </si>
+  <si>
+    <t>southtarawa</t>
+  </si>
+  <si>
+    <t>portmoresby</t>
+  </si>
+  <si>
+    <t>portvila</t>
+  </si>
+  <si>
+    <t>nukualofa</t>
+  </si>
+  <si>
+    <t>Athens boasts the Acropolis, an ancient citadel with the iconic Parthenon temple dedicated to the goddess Athena.</t>
+  </si>
+  <si>
+    <t>Budapest is famous for its thermal baths, including the Széchenyi Thermal Bath, one of the largest in Europe.</t>
+  </si>
+  <si>
+    <t>Reykjavik is the northernmost capital city in the world and offers unique opportunities to witness the Northern Lights.</t>
+  </si>
+  <si>
+    <t>Rome is home to the smallest independent state in the world, Vatican City, which is the spiritual and administrative center of the Roman Catholic Church.</t>
+  </si>
+  <si>
+    <t>Riga's historic center is famous for its Art Nouveau architecture, with over one-third of the buildings in the area displaying this style.</t>
+  </si>
+  <si>
+    <t>An interesting fact about Santiago is that despite being located in the tropics, even on the hottest summer days, the temperature rarely rises above thirty degrees.</t>
+  </si>
+  <si>
+    <t>Bogotá is located at an elevation of over 8,600 feet (2,600 meters) in the Andes Mountains, making it one of the highest capital cities in the world.</t>
+  </si>
+  <si>
+    <t>Quito is the highest capital city in the world and is famous for its well-preserved colonial old town, a UNESCO World Heritage Site.</t>
+  </si>
+  <si>
+    <t>Lima is known for its excellent cuisine and is considered the gastronomic capital of South America, offering a wide range of culinary delights.</t>
+  </si>
+  <si>
+    <t>The Eiffel Tower in Paris was originally intended to be a temporary structure for the 1889 World's Fair but became a permanent icon.</t>
+  </si>
+  <si>
+    <t>Vilnius Old Town is one of the largest preserved medieval towns in Eastern Europe and a UNESCO World Heritage site.</t>
+  </si>
+  <si>
+    <t>Monaco is the second smallest country in the world, known for its glamorous Casino de Monte-Carlo and the annual Formula 1 Grand Prix.</t>
+  </si>
+  <si>
+    <t>Podgorica is home to the Millennium Bridge, a cable-stayed bridge that changes colors at night, creating a striking visual spectacle.</t>
+  </si>
+  <si>
+    <t>Oslo is one of the world's most sustainable cities, with extensive green spaces and a strong focus on eco-friendly transportation.</t>
+  </si>
+  <si>
+    <t>The city is home to more billionaires than any other city in the world. There are around 84 billionaires living in Moscow with a combined total wealth of 367 billion dollars.</t>
+  </si>
+  <si>
+    <t>Madrid is one of Europe’s megacities, home to a staggering 3.2 million people. The only EU city with a higher population is Berlin, with 3.6 million.</t>
+  </si>
+  <si>
+    <t>Stockholm is partly known for its stunning archipelago! It consists of around 30,000 islands, islets, and rocks.</t>
+  </si>
+  <si>
+    <t>Vatican City is the smallest independent state in the world and is the spiritual and administrative center of the Roman Catholic Church.</t>
+  </si>
+  <si>
+    <t>Jerusalem is one of the oldest cities in the world and is central to the three major monotheistic religions—Judaism, Christianity, and Islam.</t>
+  </si>
+  <si>
+    <t>Tokyo's Tsukiji Fish Market, the world's largest seafood market, offers the freshest sushi and sashimi you can find.</t>
+  </si>
+  <si>
+    <t>Nur-Sultan is known for its futuristic architecture, including the Bayterek Tower, which represents a Kazakh mythological tree of life.</t>
+  </si>
+  <si>
+    <t>Kathmandu’s Swayambhunath Stupa (Monkey Temple) is not only a UNESCO World Heritage Site but also home to hundreds of monkeys considered holy by both Hindus and Buddhists.</t>
+  </si>
+  <si>
+    <t>Doha is aiming to be entirely carbon-neutral by 2030 by implementing green initiatives such as renewable energy, waste management and public transportation.</t>
+  </si>
+  <si>
+    <t>Ankara's Anıtkabir is the mausoleum of Mustafa Kemal Atatürk, the founder of modern Turkey, and a place of national significance.</t>
+  </si>
+  <si>
+    <t>Abu Dhabi's Yas Island is home to Ferrari World, a thrilling theme park with the world's fastest roller coaster.</t>
+  </si>
+  <si>
+    <t>The Long Bien Bridge in Hanoi was designed by Alexandre Gustave Eiffel, the same man who designed the Eiffel Tower in Paris and the Statue of Liberty in USA.</t>
+  </si>
+  <si>
+    <t>Monrovia, Liberia’s capital and largest city, was named after U.S. President James Monroe who was a supporter of Liberia’s establishment.</t>
+  </si>
+  <si>
+    <t>Tripoli is not only Libya’s largest city but also its capital. Its name means “Three Cities” in Greek.</t>
+  </si>
+  <si>
+    <t>greece</t>
+  </si>
+  <si>
+    <t>hungary</t>
+  </si>
+  <si>
+    <t>iceland</t>
+  </si>
+  <si>
+    <t>italy</t>
+  </si>
+  <si>
+    <t>latvia</t>
+  </si>
+  <si>
+    <t>chile</t>
+  </si>
+  <si>
+    <t>libya</t>
+  </si>
+  <si>
+    <t>liberia</t>
+  </si>
+  <si>
+    <t>vietnam</t>
+  </si>
+  <si>
+    <t>united arab emirates</t>
+  </si>
+  <si>
+    <t>turkey</t>
+  </si>
+  <si>
+    <t>thailand</t>
+  </si>
+  <si>
+    <t>qatar</t>
+  </si>
+  <si>
+    <t>nepal</t>
+  </si>
+  <si>
+    <t>kazakhstan</t>
+  </si>
+  <si>
+    <t>japan</t>
+  </si>
+  <si>
+    <t>israel</t>
+  </si>
+  <si>
+    <t>vatican city</t>
+  </si>
+  <si>
+    <t>sweden</t>
+  </si>
+  <si>
+    <t>colombia</t>
+  </si>
+  <si>
+    <t>ecuador</t>
+  </si>
+  <si>
+    <t>guyana</t>
+  </si>
+  <si>
+    <t>spain</t>
+  </si>
+  <si>
+    <t>slovakia</t>
+  </si>
+  <si>
+    <t>russia</t>
+  </si>
+  <si>
+    <t>norway</t>
+  </si>
+  <si>
+    <t>montenegro</t>
+  </si>
+  <si>
+    <t>monaco</t>
+  </si>
+  <si>
+    <t>lithuania</t>
+  </si>
+  <si>
+    <t>france</t>
+  </si>
+  <si>
+    <t>peru</t>
+  </si>
+  <si>
+    <t>athens</t>
+  </si>
+  <si>
+    <t>budapest</t>
+  </si>
+  <si>
+    <t>reykjavik</t>
+  </si>
+  <si>
+    <t>rome</t>
+  </si>
+  <si>
+    <t>riga</t>
+  </si>
+  <si>
+    <t>santiago</t>
+  </si>
+  <si>
+    <t>bogotá</t>
+  </si>
+  <si>
+    <t>quito</t>
+  </si>
+  <si>
+    <t>georgetown</t>
+  </si>
+  <si>
+    <t>lima</t>
+  </si>
+  <si>
+    <t>paris</t>
+  </si>
+  <si>
+    <t>vilnius</t>
+  </si>
+  <si>
+    <t>podgorica</t>
+  </si>
+  <si>
+    <t>oslo</t>
+  </si>
+  <si>
+    <t>moscow</t>
+  </si>
+  <si>
+    <t>bratislava</t>
+  </si>
+  <si>
+    <t>madrid</t>
+  </si>
+  <si>
+    <t>stockholm</t>
+  </si>
+  <si>
+    <t>jerusalem</t>
+  </si>
+  <si>
+    <t>tokyo</t>
+  </si>
+  <si>
+    <t>nur-sultan</t>
+  </si>
+  <si>
+    <t>kathmandu</t>
+  </si>
+  <si>
+    <t>doha</t>
+  </si>
+  <si>
+    <t>bangkok</t>
+  </si>
+  <si>
+    <t>ankara</t>
+  </si>
+  <si>
+    <t>abu dhabi</t>
+  </si>
+  <si>
+    <t>hanoi</t>
+  </si>
+  <si>
+    <t>monrovia</t>
+  </si>
+  <si>
+    <t>tripoli</t>
+  </si>
+  <si>
+    <t>Which capital city's layout was planned by American architect Walter Burley Griffin, who won an international competition for the city's design?</t>
+  </si>
+  <si>
+    <t>What capital city hosts a vibrant arts and crafts scene, where local artisans craft traditional handicrafts like pottery, woodcarvings, and woven baskets?</t>
+  </si>
+  <si>
+    <t>Which capital serves as the seat of government for Kiribati, an island nation especially susceptible to rising sea levels due to climate change?</t>
+  </si>
+  <si>
+    <t>What atoll in the Marshall Islands serves as both the capital and the largest atoll?</t>
+  </si>
+  <si>
+    <t>What city is the capital of the Federated States of Micronesia and functions as a central hub for the nation's government?</t>
+  </si>
+  <si>
+    <t>What location is considered the de facto capital of Nauru, even though the country does not officially have a capital?</t>
+  </si>
+  <si>
+    <t>Which capital city was named after the Duke of Wellington, despite him never having visited the country?</t>
+  </si>
+  <si>
+    <t>What city is the second-youngest capital in the world?</t>
+  </si>
+  <si>
+    <t>Which capital city is named after Captain John Moresby?</t>
+  </si>
+  <si>
+    <t>Which capital was initially a small village before it developed and became a capital?</t>
+  </si>
+  <si>
+    <t>What capital city is the seat of the Pacific's sole remaining monarchy?</t>
+  </si>
+  <si>
+    <t>Which capital city was named after a local tribe that inhabited the land?</t>
+  </si>
+  <si>
+    <t>Which capital is renowned for its breathtaking natural beauty and offers a range of outdoor activities for tourists?</t>
+  </si>
+  <si>
+    <t>What capital city is famous for the Acropolis?</t>
+  </si>
+  <si>
+    <t>Which capital is renowned for its thermal baths, with one of them being one of the largest in Europe?</t>
+  </si>
+  <si>
+    <t>What city holds the distinction of being the world's northernmost capital and provides unique chances to observe the Northern Lights?</t>
+  </si>
+  <si>
+    <t>Which capital city hosts the world's smallest independent state, Vatican City?</t>
+  </si>
+  <si>
+    <t>What capital city's historic center is renowned for its Art Nouveau architecture?</t>
+  </si>
+  <si>
+    <t>What capital city situated in the Andes Mountains is one of the world's highest capital cities (with an elevation exceeding 8,600 feet / 2,600 meters)?</t>
+  </si>
+  <si>
+    <t>Which capital city in the tropics experiences remarkably moderate temperatures (rarely exceeding thirty degrees)?</t>
+  </si>
+  <si>
+    <t>What capital city is renowned for its status as the world's highest capital designated as a UNESCO World Heritage Site?</t>
+  </si>
+  <si>
+    <t>Which capital city is situated below the high-tide level and is safeguarded by a seawall?</t>
+  </si>
+  <si>
+    <t>What capital city is famed for its exceptional cuisine and holds the title of the gastronomic capital of South America?</t>
+  </si>
+  <si>
+    <t>What city is home to the Eiffel Tower?</t>
+  </si>
+  <si>
+    <t>What capital city boasts one of the largest preserved medieval towns in Eastern Europe, designated as a UNESCO World Heritage site?</t>
+  </si>
+  <si>
+    <t>Which city is recognized as the second smallest country in the world?</t>
+  </si>
+  <si>
+    <t>Which capital city is the site of the Millennium Bridge, a cable-stayed bridge that undergoes color changes at night, presenting a visually striking spectacle?</t>
+  </si>
+  <si>
+    <t>What city is acknowledged as one of the world's most sustainable cities, featuring ample green spaces and a significant emphasis on eco-friendly transportation?</t>
+  </si>
+  <si>
+    <t>Which capital city hosts the largest number of billionaires in the world?</t>
+  </si>
+  <si>
+    <t>What city is considered one of Europe's megacities, housing approximately 3.2 million people, with only Berlin in the EU having a higher population?</t>
+  </si>
+  <si>
+    <t>Which capital city is celebrated for its picturesque archipelago, comprising roughly 30,000 islands, islets, and rocks?</t>
+  </si>
+  <si>
+    <t>What is the world's smallest independent state?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Which city holds central importance in three major monotheistic religions: Judaism, Christianity, and Islam?</t>
+  </si>
+  <si>
+    <t>What capital city is home to the Tsukiji Fish Market, the world's largest seafood market?</t>
+  </si>
+  <si>
+    <t>What capital city is celebrated for its futuristic architecture, featuring the Bayterek Tower?</t>
+  </si>
+  <si>
+    <t>What capital city is home to Swayambhunath Stupa, a UNESCO World Heritage Site and a sanctuary for hundreds of monkeys revered by both Hindus and Buddhists?</t>
+  </si>
+  <si>
+    <t>Which Middle Eastern capital city is striving to achieve carbon-neutrality by 2030?</t>
+  </si>
+  <si>
+    <t>What capital city features Anıtkabir, the mausoleum of Mustafa Kemal Atatürk?</t>
+  </si>
+  <si>
+    <t>Which capital city's Yas Island hosts Ferrari World, an exhilarating theme park with the world's fastest roller coaster?</t>
+  </si>
+  <si>
+    <t>What capital city is home to the Long Bien Bridge, designed by Alexandre Gustave Eiffel, who also designed the Eiffel Tower in Paris and the Statue of Liberty in the USA?</t>
+  </si>
+  <si>
+    <t>What is the capital that was named after U.S. President James Monroe?</t>
+  </si>
+  <si>
+    <t>The name of which capital means "Three Cities" in Greek?</t>
+  </si>
+  <si>
+    <t>Which capital city features the Man at Work statue (also known as Cumil), portraying a man peaking out from the sewer in the centre of old town.</t>
+  </si>
+  <si>
+    <t>Bratislava houses a Bronze sculpture of a man peeping out of the manhole called Cumil, in the center of the old town.</t>
+  </si>
+  <si>
+    <t> An interesting fact about Georgetown is that it lies below the high-tide level and is protected by a seawall with a series of canals crisscrossing the city.</t>
+  </si>
+  <si>
+    <t>Although the capital city of Thailand is known to the world as Bangkok, this is just a shortened version of the actual name, which consists of 169 characters and makes for a challenging tongue twister. The full roughly translates to:
+City of angels, great city of immortals, magnificent city of the 9 gems, seat of the king, city of royal palaces, home of gods incarnate, erected by Visvakarman at Indra's behest.</t>
+  </si>
+  <si>
+    <t>This capital's native name consists of 169 characters.</t>
   </si>
 </sst>
 </file>
@@ -684,7 +1393,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -696,11 +1405,475 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="50">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1051,21 +2224,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6DBD856-47B5-4476-9A73-818258EEBDBB}">
-  <dimension ref="A1:H58"/>
+  <dimension ref="A1:J110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScale="57" workbookViewId="0">
+      <selection activeCell="I57" sqref="I57:J58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="5" max="5" width="255.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="238.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="238.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1085,13 +2258,13 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1102,19 +2275,19 @@
         <v>65</v>
       </c>
       <c r="E2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>140</v>
+        <v>196</v>
       </c>
       <c r="H2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -1125,19 +2298,19 @@
         <v>67</v>
       </c>
       <c r="E3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>140</v>
+        <v>197</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -1148,19 +2321,19 @@
         <v>68</v>
       </c>
       <c r="E4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>140</v>
+        <v>198</v>
       </c>
       <c r="H4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1171,19 +2344,19 @@
         <v>69</v>
       </c>
       <c r="E5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F5" t="s">
         <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>140</v>
+        <v>199</v>
       </c>
       <c r="H5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1194,19 +2367,19 @@
         <v>70</v>
       </c>
       <c r="E6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>140</v>
+        <v>200</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1217,19 +2390,19 @@
         <v>71</v>
       </c>
       <c r="E7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F7" t="s">
         <v>13</v>
       </c>
-      <c r="G7" t="s">
-        <v>146</v>
+      <c r="G7" s="5" t="s">
+        <v>202</v>
       </c>
       <c r="H7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1240,19 +2413,19 @@
         <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" t="s">
-        <v>147</v>
+      <c r="G8" s="5" t="s">
+        <v>201</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1263,19 +2436,19 @@
         <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F9" t="s">
         <v>15</v>
       </c>
       <c r="G9" t="s">
-        <v>140</v>
+        <v>203</v>
       </c>
       <c r="H9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1286,19 +2459,19 @@
         <v>75</v>
       </c>
       <c r="E10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F10" t="s">
         <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="H10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1309,19 +2482,19 @@
         <v>77</v>
       </c>
       <c r="E11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11" t="s">
         <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>140</v>
+        <v>205</v>
       </c>
       <c r="H11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1332,19 +2505,19 @@
         <v>79</v>
       </c>
       <c r="E12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F12" t="s">
         <v>18</v>
       </c>
       <c r="G12" t="s">
-        <v>140</v>
+        <v>207</v>
       </c>
       <c r="H12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1355,19 +2528,19 @@
         <v>81</v>
       </c>
       <c r="E13" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F13" t="s">
         <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>140</v>
+        <v>206</v>
       </c>
       <c r="H13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1378,19 +2551,19 @@
         <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>140</v>
+        <v>208</v>
       </c>
       <c r="H14" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1401,19 +2574,19 @@
         <v>85</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F15" t="s">
         <v>21</v>
       </c>
       <c r="G15" t="s">
-        <v>140</v>
+        <v>209</v>
       </c>
       <c r="H15" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1424,19 +2597,19 @@
         <v>86</v>
       </c>
       <c r="E16" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F16" t="s">
         <v>22</v>
       </c>
       <c r="G16" t="s">
-        <v>140</v>
+        <v>210</v>
       </c>
       <c r="H16" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1447,19 +2620,19 @@
         <v>87</v>
       </c>
       <c r="E17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>211</v>
       </c>
       <c r="H17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -1470,19 +2643,19 @@
         <v>88</v>
       </c>
       <c r="E18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>140</v>
+        <v>212</v>
       </c>
       <c r="H18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -1493,19 +2666,19 @@
         <v>89</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F19" t="s">
         <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>140</v>
+        <v>213</v>
       </c>
       <c r="H19" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1516,19 +2689,19 @@
         <v>91</v>
       </c>
       <c r="E20" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F20" t="s">
         <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>140</v>
+        <v>214</v>
       </c>
       <c r="H20" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -1539,19 +2712,19 @@
         <v>92</v>
       </c>
       <c r="E21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F21" t="s">
         <v>28</v>
       </c>
       <c r="G21" t="s">
-        <v>140</v>
+        <v>215</v>
       </c>
       <c r="H21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -1562,19 +2735,19 @@
         <v>93</v>
       </c>
       <c r="E22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F22" t="s">
         <v>63</v>
       </c>
-      <c r="G22" t="s">
-        <v>198</v>
+      <c r="G22" s="5" t="s">
+        <v>216</v>
       </c>
       <c r="H22" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -1585,19 +2758,19 @@
         <v>95</v>
       </c>
       <c r="E23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F23" t="s">
         <v>64</v>
       </c>
-      <c r="G23" t="s">
-        <v>199</v>
+      <c r="G23" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="H23" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1608,19 +2781,19 @@
         <v>96</v>
       </c>
       <c r="E24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F24" t="s">
         <v>29</v>
       </c>
       <c r="G24" t="s">
-        <v>140</v>
+        <v>218</v>
       </c>
       <c r="H24" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1631,19 +2804,19 @@
         <v>97</v>
       </c>
       <c r="E25" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F25" t="s">
         <v>30</v>
       </c>
       <c r="G25" t="s">
-        <v>140</v>
+        <v>219</v>
       </c>
       <c r="H25" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -1654,19 +2827,19 @@
         <v>98</v>
       </c>
       <c r="E26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F26" t="s">
         <v>31</v>
       </c>
       <c r="G26" t="s">
-        <v>140</v>
+        <v>220</v>
       </c>
       <c r="H26" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -1677,19 +2850,19 @@
         <v>99</v>
       </c>
       <c r="E27" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F27" t="s">
         <v>32</v>
       </c>
       <c r="G27" t="s">
-        <v>140</v>
+        <v>221</v>
       </c>
       <c r="H27" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -1700,19 +2873,19 @@
         <v>100</v>
       </c>
       <c r="E28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F28" t="s">
         <v>33</v>
       </c>
       <c r="G28" t="s">
-        <v>140</v>
+        <v>222</v>
       </c>
       <c r="H28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -1723,19 +2896,19 @@
         <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F29" t="s">
         <v>102</v>
       </c>
       <c r="G29" t="s">
-        <v>140</v>
+        <v>223</v>
       </c>
       <c r="H29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -1743,22 +2916,22 @@
         <v>27</v>
       </c>
       <c r="D30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E30" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
       </c>
       <c r="G30" t="s">
-        <v>140</v>
+        <v>224</v>
       </c>
       <c r="H30" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -1766,22 +2939,22 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E31" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
       </c>
       <c r="G31" t="s">
-        <v>140</v>
+        <v>225</v>
       </c>
       <c r="H31" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -1789,22 +2962,22 @@
         <v>27</v>
       </c>
       <c r="D32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
       </c>
       <c r="G32" t="s">
-        <v>140</v>
+        <v>226</v>
       </c>
       <c r="H32" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1812,22 +2985,22 @@
         <v>27</v>
       </c>
       <c r="D33" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
       </c>
       <c r="G33" t="s">
-        <v>140</v>
+        <v>227</v>
       </c>
       <c r="H33" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1835,22 +3008,22 @@
         <v>38</v>
       </c>
       <c r="D34" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E34" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F34" t="s">
         <v>39</v>
       </c>
       <c r="G34" t="s">
-        <v>140</v>
+        <v>228</v>
       </c>
       <c r="H34" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1858,22 +3031,22 @@
         <v>38</v>
       </c>
       <c r="D35" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E35" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F35" t="s">
         <v>40</v>
       </c>
       <c r="G35" t="s">
-        <v>140</v>
+        <v>229</v>
       </c>
       <c r="H35" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1881,22 +3054,22 @@
         <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F36" t="s">
         <v>41</v>
       </c>
       <c r="G36" t="s">
-        <v>140</v>
+        <v>230</v>
       </c>
       <c r="H36" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1907,19 +3080,19 @@
         <v>42</v>
       </c>
       <c r="E37" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F37" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G37" t="s">
-        <v>140</v>
+        <v>231</v>
       </c>
       <c r="H37" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1927,22 +3100,22 @@
         <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F38" t="s">
         <v>43</v>
       </c>
       <c r="G38" t="s">
-        <v>140</v>
+        <v>232</v>
       </c>
       <c r="H38" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1950,22 +3123,22 @@
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F39" t="s">
         <v>44</v>
       </c>
-      <c r="G39" t="s">
-        <v>178</v>
+      <c r="G39" s="5" t="s">
+        <v>233</v>
       </c>
       <c r="H39" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1973,22 +3146,22 @@
         <v>38</v>
       </c>
       <c r="D40" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E40" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F40" t="s">
         <v>45</v>
       </c>
       <c r="G40" t="s">
-        <v>140</v>
+        <v>234</v>
       </c>
       <c r="H40" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1996,22 +3169,22 @@
         <v>38</v>
       </c>
       <c r="D41" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E41" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F41" t="s">
         <v>46</v>
       </c>
       <c r="G41" t="s">
-        <v>140</v>
+        <v>235</v>
       </c>
       <c r="H41" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2019,22 +3192,22 @@
         <v>38</v>
       </c>
       <c r="D42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E42" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F42" t="s">
         <v>47</v>
       </c>
       <c r="G42" t="s">
-        <v>140</v>
+        <v>236</v>
       </c>
       <c r="H42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2042,22 +3215,22 @@
         <v>38</v>
       </c>
       <c r="D43" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E43" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F43" t="s">
         <v>48</v>
       </c>
       <c r="G43" t="s">
-        <v>140</v>
+        <v>237</v>
       </c>
       <c r="H43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2065,22 +3238,22 @@
         <v>38</v>
       </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E44" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F44" t="s">
         <v>49</v>
       </c>
       <c r="G44" t="s">
-        <v>140</v>
+        <v>238</v>
       </c>
       <c r="H44" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2088,22 +3261,22 @@
         <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F45" t="s">
         <v>51</v>
       </c>
       <c r="G45" t="s">
-        <v>140</v>
+        <v>239</v>
       </c>
       <c r="H45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -2111,22 +3284,22 @@
         <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E46" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F46" t="s">
         <v>52</v>
       </c>
       <c r="G46" t="s">
-        <v>140</v>
+        <v>240</v>
       </c>
       <c r="H46" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -2134,22 +3307,22 @@
         <v>50</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="F47" t="s">
         <v>53</v>
       </c>
       <c r="G47" t="s">
-        <v>140</v>
+        <v>241</v>
       </c>
       <c r="H47" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -2157,22 +3330,22 @@
         <v>50</v>
       </c>
       <c r="D48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E48" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F48" t="s">
         <v>54</v>
       </c>
       <c r="G48" t="s">
-        <v>140</v>
+        <v>242</v>
       </c>
       <c r="H48" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -2180,22 +3353,22 @@
         <v>50</v>
       </c>
       <c r="D49" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" t="s">
+        <v>186</v>
+      </c>
+      <c r="F49" t="s">
         <v>127</v>
       </c>
-      <c r="E49" t="s">
-        <v>188</v>
-      </c>
-      <c r="F49" t="s">
-        <v>128</v>
-      </c>
       <c r="G49" t="s">
-        <v>140</v>
+        <v>243</v>
       </c>
       <c r="H49" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -2203,22 +3376,22 @@
         <v>50</v>
       </c>
       <c r="D50" t="s">
+        <v>128</v>
+      </c>
+      <c r="E50" t="s">
+        <v>187</v>
+      </c>
+      <c r="F50" t="s">
         <v>129</v>
       </c>
-      <c r="E50" t="s">
-        <v>189</v>
-      </c>
-      <c r="F50" t="s">
-        <v>102</v>
-      </c>
       <c r="G50" t="s">
-        <v>140</v>
+        <v>244</v>
       </c>
       <c r="H50" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -2226,22 +3399,22 @@
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E51" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="F51" t="s">
         <v>55</v>
       </c>
       <c r="G51" t="s">
-        <v>140</v>
+        <v>245</v>
       </c>
       <c r="H51" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2249,22 +3422,22 @@
         <v>50</v>
       </c>
       <c r="D52" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E52" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F52" t="s">
         <v>56</v>
       </c>
       <c r="G52" t="s">
-        <v>140</v>
+        <v>246</v>
       </c>
       <c r="H52" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2272,22 +3445,22 @@
         <v>50</v>
       </c>
       <c r="D53" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E53" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="F53" t="s">
         <v>57</v>
       </c>
       <c r="G53" t="s">
-        <v>140</v>
+        <v>247</v>
       </c>
       <c r="H53" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2295,22 +3468,22 @@
         <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E54" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F54" t="s">
         <v>58</v>
       </c>
       <c r="G54" t="s">
-        <v>140</v>
+        <v>248</v>
       </c>
       <c r="H54" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2318,22 +3491,22 @@
         <v>50</v>
       </c>
       <c r="D55" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E55" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F55" t="s">
         <v>59</v>
       </c>
       <c r="G55" t="s">
-        <v>140</v>
+        <v>249</v>
       </c>
       <c r="H55" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2341,22 +3514,22 @@
         <v>50</v>
       </c>
       <c r="D56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E56" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F56" t="s">
         <v>60</v>
       </c>
       <c r="G56" t="s">
-        <v>140</v>
+        <v>250</v>
       </c>
       <c r="H56" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2364,22 +3537,24 @@
         <v>50</v>
       </c>
       <c r="D57" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E57" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F57" t="s">
         <v>61</v>
       </c>
       <c r="G57" t="s">
-        <v>140</v>
+        <v>252</v>
       </c>
       <c r="H57" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2387,32 +3562,1239 @@
         <v>50</v>
       </c>
       <c r="D58" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E58" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="F58" t="s">
         <v>62</v>
       </c>
       <c r="G58" t="s">
-        <v>140</v>
+        <v>251</v>
       </c>
       <c r="H58" t="s">
         <v>62</v>
       </c>
+      <c r="I58" s="5"/>
+      <c r="J58" s="5"/>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" s="2"/>
+      <c r="C59" t="s">
+        <v>253</v>
+      </c>
+      <c r="D59" t="s">
+        <v>267</v>
+      </c>
+      <c r="E59" t="s">
+        <v>254</v>
+      </c>
+      <c r="F59" t="s">
+        <v>283</v>
+      </c>
+      <c r="G59" t="s">
+        <v>389</v>
+      </c>
+      <c r="H59" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" t="s">
+        <v>253</v>
+      </c>
+      <c r="D60" t="s">
+        <v>268</v>
+      </c>
+      <c r="E60" t="s">
+        <v>255</v>
+      </c>
+      <c r="F60" t="s">
+        <v>284</v>
+      </c>
+      <c r="G60" t="s">
+        <v>390</v>
+      </c>
+      <c r="H60" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" s="2"/>
+      <c r="C61" t="s">
+        <v>253</v>
+      </c>
+      <c r="D61" t="s">
+        <v>269</v>
+      </c>
+      <c r="E61" t="s">
+        <v>256</v>
+      </c>
+      <c r="F61" t="s">
+        <v>297</v>
+      </c>
+      <c r="G61" t="s">
+        <v>391</v>
+      </c>
+      <c r="H61" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" s="2"/>
+      <c r="C62" t="s">
+        <v>253</v>
+      </c>
+      <c r="D62" t="s">
+        <v>270</v>
+      </c>
+      <c r="E62" t="s">
+        <v>257</v>
+      </c>
+      <c r="F62" t="s">
+        <v>286</v>
+      </c>
+      <c r="G62" t="s">
+        <v>392</v>
+      </c>
+      <c r="H62" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" s="2"/>
+      <c r="C63" t="s">
+        <v>253</v>
+      </c>
+      <c r="D63" t="s">
+        <v>271</v>
+      </c>
+      <c r="E63" t="s">
+        <v>258</v>
+      </c>
+      <c r="F63" t="s">
+        <v>287</v>
+      </c>
+      <c r="G63" t="s">
+        <v>393</v>
+      </c>
+      <c r="H63" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" s="2"/>
+      <c r="C64" t="s">
+        <v>253</v>
+      </c>
+      <c r="D64" t="s">
+        <v>272</v>
+      </c>
+      <c r="E64" t="s">
+        <v>259</v>
+      </c>
+      <c r="F64" t="s">
+        <v>288</v>
+      </c>
+      <c r="G64" t="s">
+        <v>394</v>
+      </c>
+      <c r="H64" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" t="s">
+        <v>253</v>
+      </c>
+      <c r="D65" t="s">
+        <v>273</v>
+      </c>
+      <c r="E65" t="s">
+        <v>260</v>
+      </c>
+      <c r="F65" t="s">
+        <v>289</v>
+      </c>
+      <c r="G65" t="s">
+        <v>395</v>
+      </c>
+      <c r="H65" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" t="s">
+        <v>253</v>
+      </c>
+      <c r="D66" t="s">
+        <v>274</v>
+      </c>
+      <c r="E66" t="s">
+        <v>261</v>
+      </c>
+      <c r="F66" t="s">
+        <v>290</v>
+      </c>
+      <c r="G66" t="s">
+        <v>396</v>
+      </c>
+      <c r="H66" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" t="s">
+        <v>253</v>
+      </c>
+      <c r="D67" t="s">
+        <v>275</v>
+      </c>
+      <c r="E67" t="s">
+        <v>262</v>
+      </c>
+      <c r="F67" t="s">
+        <v>298</v>
+      </c>
+      <c r="G67" t="s">
+        <v>397</v>
+      </c>
+      <c r="H67" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" s="2"/>
+      <c r="C68" t="s">
+        <v>253</v>
+      </c>
+      <c r="D68" t="s">
+        <v>276</v>
+      </c>
+      <c r="E68" t="s">
+        <v>263</v>
+      </c>
+      <c r="F68" t="s">
+        <v>292</v>
+      </c>
+      <c r="G68" t="s">
+        <v>398</v>
+      </c>
+      <c r="H68" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" s="2"/>
+      <c r="C69" t="s">
+        <v>253</v>
+      </c>
+      <c r="D69" t="s">
+        <v>277</v>
+      </c>
+      <c r="E69" t="s">
+        <v>281</v>
+      </c>
+      <c r="F69" t="s">
+        <v>293</v>
+      </c>
+      <c r="G69" t="s">
+        <v>282</v>
+      </c>
+      <c r="H69" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+      <c r="B70" s="2"/>
+      <c r="C70" t="s">
+        <v>253</v>
+      </c>
+      <c r="D70" t="s">
+        <v>278</v>
+      </c>
+      <c r="E70" t="s">
+        <v>264</v>
+      </c>
+      <c r="F70" t="s">
+        <v>300</v>
+      </c>
+      <c r="G70" t="s">
+        <v>399</v>
+      </c>
+      <c r="H70" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="B71" s="2"/>
+      <c r="C71" t="s">
+        <v>253</v>
+      </c>
+      <c r="D71" t="s">
+        <v>279</v>
+      </c>
+      <c r="E71" t="s">
+        <v>265</v>
+      </c>
+      <c r="F71" t="s">
+        <v>295</v>
+      </c>
+      <c r="G71" t="s">
+        <v>400</v>
+      </c>
+      <c r="H71" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" t="s">
+        <v>253</v>
+      </c>
+      <c r="D72" t="s">
+        <v>280</v>
+      </c>
+      <c r="E72" t="s">
+        <v>266</v>
+      </c>
+      <c r="F72" t="s">
+        <v>299</v>
+      </c>
+      <c r="G72" t="s">
+        <v>401</v>
+      </c>
+      <c r="H72" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+      <c r="C73" t="s">
+        <v>27</v>
+      </c>
+      <c r="D73" t="s">
+        <v>329</v>
+      </c>
+      <c r="E73" t="s">
+        <v>301</v>
+      </c>
+      <c r="F73" t="s">
+        <v>360</v>
+      </c>
+      <c r="G73" t="s">
+        <v>402</v>
+      </c>
+      <c r="H73" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="C74" t="s">
+        <v>27</v>
+      </c>
+      <c r="D74" t="s">
+        <v>330</v>
+      </c>
+      <c r="E74" t="s">
+        <v>302</v>
+      </c>
+      <c r="F74" t="s">
+        <v>361</v>
+      </c>
+      <c r="G74" t="s">
+        <v>403</v>
+      </c>
+      <c r="H74" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="C75" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" t="s">
+        <v>331</v>
+      </c>
+      <c r="E75" t="s">
+        <v>303</v>
+      </c>
+      <c r="F75" t="s">
+        <v>362</v>
+      </c>
+      <c r="G75" t="s">
+        <v>404</v>
+      </c>
+      <c r="H75" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="C76" t="s">
+        <v>27</v>
+      </c>
+      <c r="D76" t="s">
+        <v>332</v>
+      </c>
+      <c r="E76" t="s">
+        <v>304</v>
+      </c>
+      <c r="F76" t="s">
+        <v>363</v>
+      </c>
+      <c r="G76" t="s">
+        <v>405</v>
+      </c>
+      <c r="H76" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="C77" t="s">
+        <v>27</v>
+      </c>
+      <c r="D77" t="s">
+        <v>333</v>
+      </c>
+      <c r="E77" t="s">
+        <v>305</v>
+      </c>
+      <c r="F77" t="s">
+        <v>364</v>
+      </c>
+      <c r="G77" t="s">
+        <v>406</v>
+      </c>
+      <c r="H77" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+      <c r="C78" t="s">
+        <v>7</v>
+      </c>
+      <c r="D78" t="s">
+        <v>334</v>
+      </c>
+      <c r="E78" t="s">
+        <v>306</v>
+      </c>
+      <c r="F78" t="s">
+        <v>365</v>
+      </c>
+      <c r="G78" t="s">
+        <v>408</v>
+      </c>
+      <c r="H78" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+      <c r="C79" t="s">
+        <v>7</v>
+      </c>
+      <c r="D79" t="s">
+        <v>348</v>
+      </c>
+      <c r="E79" t="s">
+        <v>307</v>
+      </c>
+      <c r="F79" t="s">
+        <v>366</v>
+      </c>
+      <c r="G79" t="s">
+        <v>407</v>
+      </c>
+      <c r="H79" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="C80" t="s">
+        <v>7</v>
+      </c>
+      <c r="D80" t="s">
+        <v>349</v>
+      </c>
+      <c r="E80" t="s">
+        <v>308</v>
+      </c>
+      <c r="F80" t="s">
+        <v>367</v>
+      </c>
+      <c r="G80" t="s">
+        <v>409</v>
+      </c>
+      <c r="H80" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+      <c r="C81" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" t="s">
+        <v>350</v>
+      </c>
+      <c r="E81" t="s">
+        <v>433</v>
+      </c>
+      <c r="F81" t="s">
+        <v>368</v>
+      </c>
+      <c r="G81" t="s">
+        <v>410</v>
+      </c>
+      <c r="H81" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A82" s="2">
+        <v>81</v>
+      </c>
+      <c r="C82" t="s">
+        <v>7</v>
+      </c>
+      <c r="D82" t="s">
+        <v>359</v>
+      </c>
+      <c r="E82" t="s">
+        <v>309</v>
+      </c>
+      <c r="F82" t="s">
+        <v>369</v>
+      </c>
+      <c r="G82" t="s">
+        <v>411</v>
+      </c>
+      <c r="H82" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="C83" t="s">
+        <v>27</v>
+      </c>
+      <c r="D83" t="s">
+        <v>358</v>
+      </c>
+      <c r="E83" t="s">
+        <v>310</v>
+      </c>
+      <c r="F83" t="s">
+        <v>370</v>
+      </c>
+      <c r="G83" t="s">
+        <v>412</v>
+      </c>
+      <c r="H83" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="C84" t="s">
+        <v>27</v>
+      </c>
+      <c r="D84" t="s">
+        <v>357</v>
+      </c>
+      <c r="E84" t="s">
+        <v>311</v>
+      </c>
+      <c r="F84" t="s">
+        <v>371</v>
+      </c>
+      <c r="G84" t="s">
+        <v>413</v>
+      </c>
+      <c r="H84" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A85" s="2">
+        <v>84</v>
+      </c>
+      <c r="C85" t="s">
+        <v>27</v>
+      </c>
+      <c r="D85" t="s">
+        <v>356</v>
+      </c>
+      <c r="E85" t="s">
+        <v>312</v>
+      </c>
+      <c r="F85" t="s">
+        <v>356</v>
+      </c>
+      <c r="G85" t="s">
+        <v>414</v>
+      </c>
+      <c r="H85" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
+      <c r="C86" t="s">
+        <v>27</v>
+      </c>
+      <c r="D86" t="s">
+        <v>355</v>
+      </c>
+      <c r="E86" t="s">
+        <v>313</v>
+      </c>
+      <c r="F86" t="s">
+        <v>372</v>
+      </c>
+      <c r="G86" t="s">
+        <v>415</v>
+      </c>
+      <c r="H86" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A87" s="2">
+        <v>86</v>
+      </c>
+      <c r="C87" t="s">
+        <v>27</v>
+      </c>
+      <c r="D87" t="s">
+        <v>354</v>
+      </c>
+      <c r="E87" t="s">
+        <v>314</v>
+      </c>
+      <c r="F87" t="s">
+        <v>373</v>
+      </c>
+      <c r="G87" t="s">
+        <v>416</v>
+      </c>
+      <c r="H87" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A88" s="2">
+        <v>87</v>
+      </c>
+      <c r="C88" t="s">
+        <v>27</v>
+      </c>
+      <c r="D88" t="s">
+        <v>353</v>
+      </c>
+      <c r="E88" t="s">
+        <v>315</v>
+      </c>
+      <c r="F88" t="s">
+        <v>374</v>
+      </c>
+      <c r="G88" t="s">
+        <v>417</v>
+      </c>
+      <c r="H88" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A89" s="6">
+        <v>88</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E89" s="5" t="s">
+        <v>432</v>
+      </c>
+      <c r="F89" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="G89" s="5" t="s">
+        <v>431</v>
+      </c>
+      <c r="H89" s="5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A90" s="2">
+        <v>89</v>
+      </c>
+      <c r="C90" t="s">
+        <v>27</v>
+      </c>
+      <c r="D90" t="s">
+        <v>351</v>
+      </c>
+      <c r="E90" t="s">
+        <v>316</v>
+      </c>
+      <c r="F90" t="s">
+        <v>376</v>
+      </c>
+      <c r="G90" t="s">
+        <v>418</v>
+      </c>
+      <c r="H90" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A91" s="2">
+        <v>90</v>
+      </c>
+      <c r="C91" t="s">
+        <v>27</v>
+      </c>
+      <c r="D91" t="s">
+        <v>347</v>
+      </c>
+      <c r="E91" t="s">
+        <v>317</v>
+      </c>
+      <c r="F91" t="s">
+        <v>377</v>
+      </c>
+      <c r="G91" t="s">
+        <v>419</v>
+      </c>
+      <c r="H91" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A92" s="2">
+        <v>91</v>
+      </c>
+      <c r="C92" t="s">
+        <v>27</v>
+      </c>
+      <c r="D92" t="s">
+        <v>346</v>
+      </c>
+      <c r="E92" t="s">
+        <v>318</v>
+      </c>
+      <c r="F92" t="s">
+        <v>346</v>
+      </c>
+      <c r="G92" t="s">
+        <v>420</v>
+      </c>
+      <c r="H92" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A93" s="2">
+        <v>92</v>
+      </c>
+      <c r="C93" t="s">
+        <v>38</v>
+      </c>
+      <c r="D93" t="s">
+        <v>345</v>
+      </c>
+      <c r="E93" t="s">
+        <v>319</v>
+      </c>
+      <c r="F93" t="s">
+        <v>378</v>
+      </c>
+      <c r="G93" t="s">
+        <v>421</v>
+      </c>
+      <c r="H93" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A94" s="2">
+        <v>93</v>
+      </c>
+      <c r="C94" t="s">
+        <v>38</v>
+      </c>
+      <c r="D94" t="s">
+        <v>344</v>
+      </c>
+      <c r="E94" t="s">
+        <v>320</v>
+      </c>
+      <c r="F94" t="s">
+        <v>379</v>
+      </c>
+      <c r="G94" t="s">
+        <v>422</v>
+      </c>
+      <c r="H94" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A95" s="2">
+        <v>94</v>
+      </c>
+      <c r="C95" t="s">
+        <v>38</v>
+      </c>
+      <c r="D95" t="s">
+        <v>343</v>
+      </c>
+      <c r="E95" t="s">
+        <v>321</v>
+      </c>
+      <c r="F95" t="s">
+        <v>380</v>
+      </c>
+      <c r="G95" t="s">
+        <v>423</v>
+      </c>
+      <c r="H95" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A96" s="2">
+        <v>95</v>
+      </c>
+      <c r="C96" t="s">
+        <v>38</v>
+      </c>
+      <c r="D96" t="s">
+        <v>342</v>
+      </c>
+      <c r="E96" t="s">
+        <v>322</v>
+      </c>
+      <c r="F96" t="s">
+        <v>381</v>
+      </c>
+      <c r="G96" t="s">
+        <v>424</v>
+      </c>
+      <c r="H96" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A97" s="2">
+        <v>96</v>
+      </c>
+      <c r="C97" t="s">
+        <v>38</v>
+      </c>
+      <c r="D97" t="s">
+        <v>341</v>
+      </c>
+      <c r="E97" t="s">
+        <v>323</v>
+      </c>
+      <c r="F97" t="s">
+        <v>382</v>
+      </c>
+      <c r="G97" t="s">
+        <v>425</v>
+      </c>
+      <c r="H97" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A98" s="2">
+        <v>97</v>
+      </c>
+      <c r="C98" t="s">
+        <v>38</v>
+      </c>
+      <c r="D98" t="s">
+        <v>340</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="F98" t="s">
+        <v>383</v>
+      </c>
+      <c r="G98" t="s">
+        <v>435</v>
+      </c>
+      <c r="H98" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A99" s="2">
+        <v>98</v>
+      </c>
+      <c r="C99" t="s">
+        <v>38</v>
+      </c>
+      <c r="D99" t="s">
+        <v>339</v>
+      </c>
+      <c r="E99" t="s">
+        <v>324</v>
+      </c>
+      <c r="F99" t="s">
+        <v>384</v>
+      </c>
+      <c r="G99" t="s">
+        <v>426</v>
+      </c>
+      <c r="H99" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A100" s="2">
+        <v>99</v>
+      </c>
+      <c r="C100" t="s">
+        <v>38</v>
+      </c>
+      <c r="D100" t="s">
+        <v>338</v>
+      </c>
+      <c r="E100" t="s">
+        <v>325</v>
+      </c>
+      <c r="F100" t="s">
+        <v>385</v>
+      </c>
+      <c r="G100" t="s">
+        <v>427</v>
+      </c>
+      <c r="H100" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A101" s="2">
+        <v>100</v>
+      </c>
+      <c r="C101" t="s">
+        <v>38</v>
+      </c>
+      <c r="D101" t="s">
+        <v>337</v>
+      </c>
+      <c r="E101" t="s">
+        <v>326</v>
+      </c>
+      <c r="F101" t="s">
+        <v>386</v>
+      </c>
+      <c r="G101" t="s">
+        <v>428</v>
+      </c>
+      <c r="H101" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A102" s="2">
+        <v>101</v>
+      </c>
+      <c r="C102" t="s">
+        <v>50</v>
+      </c>
+      <c r="D102" t="s">
+        <v>336</v>
+      </c>
+      <c r="E102" t="s">
+        <v>327</v>
+      </c>
+      <c r="F102" t="s">
+        <v>387</v>
+      </c>
+      <c r="G102" t="s">
+        <v>429</v>
+      </c>
+      <c r="H102" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A103" s="2">
+        <v>102</v>
+      </c>
+      <c r="C103" t="s">
+        <v>50</v>
+      </c>
+      <c r="D103" t="s">
+        <v>335</v>
+      </c>
+      <c r="E103" t="s">
+        <v>328</v>
+      </c>
+      <c r="F103" t="s">
+        <v>388</v>
+      </c>
+      <c r="G103" t="s">
+        <v>430</v>
+      </c>
+      <c r="H103" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A104" s="2"/>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A105" s="2"/>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A106" s="2"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A107" s="2"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A108" s="2"/>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A109" s="2"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A110" s="2"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="H2:H20">
+    <cfRule type="duplicateValues" dxfId="49" priority="49"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H21:H33">
+    <cfRule type="duplicateValues" dxfId="48" priority="48"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34:H44">
+    <cfRule type="duplicateValues" dxfId="47" priority="47"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H45:H58 I58">
+    <cfRule type="duplicateValues" dxfId="46" priority="46"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G69">
+    <cfRule type="duplicateValues" dxfId="44" priority="45"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H59:H72">
+    <cfRule type="duplicateValues" dxfId="43" priority="44"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F59:F72 G59:G68 G70:G103">
+    <cfRule type="duplicateValues" dxfId="42" priority="43"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H73:H75">
+    <cfRule type="duplicateValues" dxfId="41" priority="42"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H76:H77">
+    <cfRule type="duplicateValues" dxfId="40" priority="41"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H78:H81">
+    <cfRule type="duplicateValues" dxfId="39" priority="40"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H82">
+    <cfRule type="duplicateValues" dxfId="38" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H83">
+    <cfRule type="duplicateValues" dxfId="37" priority="38"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H84">
+    <cfRule type="duplicateValues" dxfId="36" priority="37"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H85:H86">
+    <cfRule type="duplicateValues" dxfId="35" priority="36"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H87">
+    <cfRule type="duplicateValues" dxfId="34" priority="35"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H88">
+    <cfRule type="duplicateValues" dxfId="33" priority="34"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H89">
+    <cfRule type="duplicateValues" dxfId="32" priority="33"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H90:H91">
+    <cfRule type="duplicateValues" dxfId="31" priority="32"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H92">
+    <cfRule type="duplicateValues" dxfId="30" priority="31"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H93:H94">
+    <cfRule type="duplicateValues" dxfId="29" priority="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H95">
+    <cfRule type="duplicateValues" dxfId="28" priority="29"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H96">
+    <cfRule type="duplicateValues" dxfId="27" priority="28"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H97">
+    <cfRule type="duplicateValues" dxfId="26" priority="27"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H98">
+    <cfRule type="duplicateValues" dxfId="25" priority="26"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H99">
+    <cfRule type="duplicateValues" dxfId="24" priority="25"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H100">
+    <cfRule type="duplicateValues" dxfId="23" priority="24"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H101">
+    <cfRule type="duplicateValues" dxfId="22" priority="23"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H102:H103">
+    <cfRule type="duplicateValues" dxfId="21" priority="22"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F73:F75">
+    <cfRule type="duplicateValues" dxfId="20" priority="21"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F76:F77">
+    <cfRule type="duplicateValues" dxfId="19" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F78:F81">
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F82">
+    <cfRule type="duplicateValues" dxfId="17" priority="18"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F83">
+    <cfRule type="duplicateValues" dxfId="16" priority="17"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F84">
+    <cfRule type="duplicateValues" dxfId="15" priority="16"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F85:F86">
+    <cfRule type="duplicateValues" dxfId="14" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F87">
+    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F88">
+    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F89">
+    <cfRule type="duplicateValues" dxfId="11" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F90:F91">
+    <cfRule type="duplicateValues" dxfId="10" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F92">
+    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F93:F94">
+    <cfRule type="duplicateValues" dxfId="8" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F95">
+    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F96">
+    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F97">
+    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F98">
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F99">
     <cfRule type="duplicateValues" dxfId="3" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H21:H33">
+  <conditionalFormatting sqref="F100">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H34:H44">
+  <conditionalFormatting sqref="F101">
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H45:H58">
+  <conditionalFormatting sqref="F102:F103">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>